<commit_message>
ADMIN - S - Start of table
</commit_message>
<xml_diff>
--- a/taakverdeling.xlsx
+++ b/taakverdeling.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bachelor\23-24\SEM3\SEP\sep2324-gent-ep3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF778D47-1FCE-4DBC-8105-8455FBE2953D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,49 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>TAAK</t>
+  </si>
+  <si>
+    <t>UITGEVOERD DOOR</t>
+  </si>
+  <si>
+    <t>Base repo aanmaken en opvullen</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>DNS script providen en aanpassen</t>
+  </si>
+  <si>
+    <t>Jelle</t>
+  </si>
+  <si>
+    <t>Changes aan base scripts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -37,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -45,14 +88,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +419,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to track file and added EP3 excercise rules
</commit_message>
<xml_diff>
--- a/taakverdeling.xlsx
+++ b/taakverdeling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bachelor\23-24\SEM3\SEP\sep2324-gent-ep3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF778D47-1FCE-4DBC-8105-8455FBE2953D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FD07C8-A49C-47E6-B9C9-742312A3661B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,22 +33,22 @@
     <t>UITGEVOERD DOOR</t>
   </si>
   <si>
-    <t>Base repo aanmaken en opvullen</t>
-  </si>
-  <si>
     <t>Thomas</t>
   </si>
   <si>
-    <t>DNS script providen en aanpassen</t>
-  </si>
-  <si>
     <t>Jelle</t>
   </si>
   <si>
-    <t>Changes aan base scripts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas </t>
+    <t>EP2 REPO van eigen groep gekopieerd naar nieuwe repo.</t>
+  </si>
+  <si>
+    <t>DNS script EP2 met kleine aanpassingen.</t>
+  </si>
+  <si>
+    <t>Fysieke testdag op school, focus op totaal test, troubleshooting netwerk.</t>
+  </si>
+  <si>
+    <t>Thomas en Jelle</t>
   </si>
 </sst>
 </file>
@@ -131,14 +131,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -423,12 +421,12 @@
   <dimension ref="B2:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="130.85546875" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -441,156 +439,124 @@
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="5"/>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="5"/>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="5"/>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="5"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="5"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="5"/>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="5"/>
-      <c r="C37" s="3"/>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>